<commit_message>
fixing logic of overall score kpi
</commit_message>
<xml_diff>
--- a/Projects/JRIJP/Data/jrijp_config_sample.xlsx
+++ b/Projects/JRIJP/Data/jrijp_config_sample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t xml:space="preserve">product group name</t>
   </si>
@@ -52,34 +52,28 @@
     <t xml:space="preserve">Group_1</t>
   </si>
   <si>
+    <t xml:space="preserve">exclude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group_2</t>
+  </si>
+  <si>
     <t xml:space="preserve">4901872061280, 4901872099122, 4901872963461</t>
   </si>
   <si>
     <t xml:space="preserve">1,2</t>
   </si>
   <si>
-    <t xml:space="preserve">exclude</t>
-  </si>
-  <si>
     <t xml:space="preserve">Secondary(Side net), Secondary Self Skin Care</t>
   </si>
   <si>
-    <t xml:space="preserve">Group_2</t>
+    <t xml:space="preserve">Group_3</t>
   </si>
   <si>
     <t xml:space="preserve">4901872963300, 4901872963461, 4901872049882, 4987241155736</t>
   </si>
   <si>
     <t xml:space="preserve">5,6,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Group_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4987241155729, 4514254054390, 4971710393095</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6,7</t>
   </si>
   <si>
     <t xml:space="preserve">Group_4</t>
@@ -240,22 +234,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="27.7449392712551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.3522267206478"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="42.2064777327935"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="43.7044534412956"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9"/>
     <col collapsed="false" hidden="false" max="1023" min="10" style="1" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.57085020242915"/>
@@ -290,28 +284,26 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="6" t="n">
+        <v>4987241155729</v>
+      </c>
+      <c r="C2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="G2" s="5"/>
       <c r="H2" s="7" t="n">
         <v>43101</v>
       </c>
@@ -319,27 +311,27 @@
         <v>43850</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>13</v>
       </c>
       <c r="H3" s="7" t="n">
         <v>43101</v>
@@ -348,27 +340,27 @@
         <v>43850</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="E4" s="5" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H4" s="7" t="n">
         <v>43101</v>
@@ -379,22 +371,22 @@
     </row>
     <row r="5" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" s="5" t="n">
         <v>3</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E5" s="5" t="n">
         <v>1</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="7" t="n">
@@ -404,6 +396,7 @@
         <v>43850</v>
       </c>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>